<commit_message>
Updated the Configuration File for Department Creation
</commit_message>
<xml_diff>
--- a/DepartmentCreation.xlsx
+++ b/DepartmentCreation.xlsx
@@ -423,7 +423,7 @@
     <t>ACN DOP DEP123456</t>
   </si>
   <si>
-    <t>ACN DOP DEP DevOps</t>
+    <t>ACN DOP DEP DevOps Sample123456</t>
   </si>
 </sst>
 </file>
@@ -17035,7 +17035,7 @@
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="83" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>